<commit_message>
added overall week num
</commit_message>
<xml_diff>
--- a/Draft project plan.xlsx
+++ b/Draft project plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\Admin-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA3EC88-0033-41B6-A74C-05A77E8CD71C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A714EFF4-D759-42BC-951B-201F727F6FC2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{B4C48C62-75A8-4245-BB0C-22D26E733F0A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Research</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Month</t>
   </si>
   <si>
-    <t>Week (W/C)</t>
-  </si>
-  <si>
     <t>5 (29th)</t>
   </si>
   <si>
@@ -217,6 +214,12 @@
   </si>
   <si>
     <t xml:space="preserve">Peer review 2  - 3rd </t>
+  </si>
+  <si>
+    <t>Official week num</t>
+  </si>
+  <si>
+    <t>Week num  (W/C)</t>
   </si>
 </sst>
 </file>
@@ -365,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -383,6 +386,30 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -396,27 +423,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -761,15 +767,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C76B9B-D484-4B7A-BF3D-26BB456E23D9}">
-  <dimension ref="A2:AC18"/>
+  <dimension ref="A2:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
@@ -782,199 +788,267 @@
       <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+    </row>
+    <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="9">
+        <v>5</v>
+      </c>
+      <c r="D3" s="9">
+        <v>6</v>
+      </c>
+      <c r="E3" s="9">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9">
+        <v>8</v>
+      </c>
+      <c r="G3" s="9">
+        <v>9</v>
+      </c>
+      <c r="H3" s="9">
+        <v>10</v>
+      </c>
+      <c r="I3" s="9">
+        <v>11</v>
+      </c>
+      <c r="J3" s="9">
+        <v>12</v>
+      </c>
+      <c r="K3" s="9">
         <v>13</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14" t="s">
+      <c r="L3" s="9">
+        <v>14</v>
+      </c>
+      <c r="M3" s="9">
+        <v>15</v>
+      </c>
+      <c r="N3" s="9">
+        <v>16</v>
+      </c>
+      <c r="O3" s="9">
+        <v>17</v>
+      </c>
+      <c r="P3" s="9">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>19</v>
+      </c>
+      <c r="R3" s="9">
         <v>20</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14" t="s">
+      <c r="S3" s="9">
+        <v>21</v>
+      </c>
+      <c r="T3" s="9">
+        <v>22</v>
+      </c>
+      <c r="U3" s="9">
+        <v>23</v>
+      </c>
+      <c r="V3" s="9">
+        <v>24</v>
+      </c>
+      <c r="W3" s="9">
         <v>25</v>
       </c>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14" t="s">
+      <c r="X3" s="9">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>28</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>29</v>
+      </c>
+      <c r="AB3" s="9">
         <v>30</v>
       </c>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14" t="s">
+      <c r="AC3" s="9">
         <v>31</v>
       </c>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-    </row>
-    <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="8" t="s">
+      <c r="H4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="L4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="J5" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="X3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB3" s="8" t="s">
+      <c r="K5" s="16"/>
+      <c r="AC5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AC3" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="J4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="20"/>
-      <c r="AC4" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="AC5" s="15"/>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="AC6" s="11"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="AC6" s="15"/>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="AC7" s="15"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="AC7" s="11"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="19"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="AC8" s="11"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="AC8" s="15"/>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -987,122 +1061,140 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="AC9" s="15"/>
+      <c r="AC9" s="11"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="20"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="AC10" s="11"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4"/>
-      <c r="AB10" s="4"/>
-      <c r="AC10" s="15"/>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="E11" s="5"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4"/>
+      <c r="AC11" s="11"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J12" s="16" t="s">
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="J13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="17"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" s="18"/>
-    </row>
-    <row r="14" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="O13" s="14"/>
+    </row>
+    <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="T15" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="U15" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="X15" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="T14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="U14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="X14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC14" s="9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="X15" s="9"/>
-      <c r="AC15" s="9"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="X16" s="9"/>
-      <c r="AC16" s="9"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="X17" s="9"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
+      <c r="A16" s="21"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="AC16" s="17"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="AC17" s="17"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="T15:T19"/>
+    <mergeCell ref="U15:U19"/>
+    <mergeCell ref="X15:X18"/>
+    <mergeCell ref="AC15:AC17"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="A15:A19"/>
     <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="AC4:AC10"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AC5:AC11"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="J4:K11"/>
+    <mergeCell ref="J5:K12"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="U2:X2"/>
-    <mergeCell ref="T14:T18"/>
-    <mergeCell ref="U14:U18"/>
-    <mergeCell ref="X14:X17"/>
-    <mergeCell ref="AC14:AC16"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="A14:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1127,47 +1219,47 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,22 +1267,22 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1198,7 +1290,7 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding agenda, edits to contract and project plan
Contract was spelling error, plan added tasks
</commit_message>
<xml_diff>
--- a/Draft project plan.xlsx
+++ b/Draft project plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Documents\GitHub\Admin-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A714EFF4-D759-42BC-951B-201F727F6FC2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E5F170-68BE-46F9-B681-D25E1D570282}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{B4C48C62-75A8-4245-BB0C-22D26E733F0A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Gantt chart" sheetId="1" r:id="rId1"/>
     <sheet name="Details for each" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="179021" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Research</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Web design needs</t>
   </si>
   <si>
-    <t>App layout design (UI)</t>
-  </si>
-  <si>
     <t>Specification</t>
   </si>
   <si>
@@ -220,6 +217,15 @@
   </si>
   <si>
     <t>Week num  (W/C)</t>
+  </si>
+  <si>
+    <t>App layout design (UI) Storyboard</t>
+  </si>
+  <si>
+    <t>requirements</t>
+  </si>
+  <si>
+    <t>criteria</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -388,6 +394,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -769,9 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27C76B9B-D484-4B7A-BF3D-26BB456E23D9}">
   <dimension ref="A2:AC19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,48 +798,48 @@
       <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10" t="s">
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10" t="s">
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="10"/>
-      <c r="Y2" s="10" t="s">
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
     </row>
     <row r="3" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="9">
         <v>5</v>
@@ -915,7 +925,7 @@
     </row>
     <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>7</v>
@@ -1000,55 +1010,55 @@
       </c>
     </row>
     <row r="5" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="J5" s="16" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="J5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="AC5" s="11" t="s">
+      <c r="K5" s="18"/>
+      <c r="AC5" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="20"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="AC6" s="11"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="AC6" s="13"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="21" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="AC7" s="11"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="AC7" s="13"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="21"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="AC8" s="11"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="AC8" s="13"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -1061,12 +1071,12 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
-      <c r="AC9" s="11"/>
+      <c r="AC9" s="13"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="A10" s="22"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -1079,97 +1089,97 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
-      <c r="AC10" s="11"/>
+      <c r="AC10" s="13"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="5"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-      <c r="AC11" s="11"/>
+      <c r="AC11" s="13"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="J13" s="12" t="s">
+      <c r="J13" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="N13" s="13" t="s">
+      <c r="N13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O13" s="14"/>
+      <c r="O13" s="16"/>
     </row>
     <row r="15" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="T15" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="U15" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="X15" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC15" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="T15" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="U15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="X15" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC15" s="17" t="s">
-        <v>60</v>
-      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="T16" s="17"/>
-      <c r="U16" s="17"/>
-      <c r="X16" s="17"/>
-      <c r="AC16" s="17"/>
+      <c r="A16" s="23"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="X16" s="19"/>
+      <c r="AC16" s="19"/>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="AC17" s="17"/>
+      <c r="A17" s="23"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="AC17" s="19"/>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17"/>
-      <c r="X18" s="17"/>
+      <c r="A18" s="23"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="X18" s="19"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="17"/>
+      <c r="A19" s="23"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -1191,10 +1201,10 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="H2:L2"/>
-    <mergeCell ref="J5:K12"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:T2"/>
     <mergeCell ref="U2:X2"/>
+    <mergeCell ref="J5:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1202,19 +1212,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B058B51-C5B5-41BD-9C91-0E4A6CB7E516}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1222,78 +1233,85 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>51</v>
+      <c r="B17" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>